<commit_message>
Reorganized the like and lock button
</commit_message>
<xml_diff>
--- a/scripts/story.xlsx
+++ b/scripts/story.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/dev/chimple/maui/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43750CA0-07B2-D14B-949B-CDA5F8E66698}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C2903C-6F60-EF4C-9DC4-6E558A385637}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="460" windowWidth="20520" windowHeight="16160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8280" yWindow="460" windowWidth="20520" windowHeight="16160" firstSheet="81" activeTab="88" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24752" sheetId="3" r:id="rId1"/>
@@ -100,30 +100,26 @@
     <sheet name="22567" sheetId="87" r:id="rId85"/>
     <sheet name="6476" sheetId="88" r:id="rId86"/>
     <sheet name="23308" sheetId="89" r:id="rId87"/>
-    <sheet name="7780" sheetId="90" r:id="rId88"/>
-    <sheet name="8706" sheetId="91" r:id="rId89"/>
-    <sheet name="13153" sheetId="92" r:id="rId90"/>
-    <sheet name="21841" sheetId="93" r:id="rId91"/>
-    <sheet name="18804" sheetId="94" r:id="rId92"/>
-    <sheet name="20440" sheetId="95" r:id="rId93"/>
-    <sheet name="21140" sheetId="96" r:id="rId94"/>
-    <sheet name="23158" sheetId="97" r:id="rId95"/>
-    <sheet name="2335" sheetId="98" r:id="rId96"/>
-    <sheet name="2209" sheetId="99" r:id="rId97"/>
-    <sheet name="20022" sheetId="100" r:id="rId98"/>
-    <sheet name="10161" sheetId="101" r:id="rId99"/>
-    <sheet name="22004" sheetId="102" r:id="rId100"/>
-    <sheet name="24751" sheetId="103" r:id="rId101"/>
-    <sheet name="15939" sheetId="104" r:id="rId102"/>
-    <sheet name="21863" sheetId="105" r:id="rId103"/>
-    <sheet name="23035" sheetId="106" r:id="rId104"/>
+    <sheet name="21841" sheetId="93" r:id="rId88"/>
+    <sheet name="20440" sheetId="95" r:id="rId89"/>
+    <sheet name="21140" sheetId="96" r:id="rId90"/>
+    <sheet name="23158" sheetId="97" r:id="rId91"/>
+    <sheet name="2335" sheetId="98" r:id="rId92"/>
+    <sheet name="2209" sheetId="99" r:id="rId93"/>
+    <sheet name="20022" sheetId="100" r:id="rId94"/>
+    <sheet name="10161" sheetId="101" r:id="rId95"/>
+    <sheet name="22004" sheetId="102" r:id="rId96"/>
+    <sheet name="24751" sheetId="103" r:id="rId97"/>
+    <sheet name="15939" sheetId="104" r:id="rId98"/>
+    <sheet name="21863" sheetId="105" r:id="rId99"/>
+    <sheet name="23035" sheetId="106" r:id="rId100"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5354" uniqueCount="3207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5226" uniqueCount="3178">
   <si>
     <t>type</t>
   </si>
@@ -10773,55 +10769,6 @@
 http://cae.ukzn.ac.za/resources/seedbooks.aspx</t>
   </si>
   <si>
-    <t>Kifungua Kinywa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fatma Baraka
-Cathy Feek</t>
-  </si>
-  <si>
-    <t>Babangu anapenda sana uji wa mahindi.</t>
-  </si>
-  <si>
-    <t>Mimi napendelea uji wa wimbi.</t>
-  </si>
-  <si>
-    <t>Babangu anapenda kahawa.</t>
-  </si>
-  <si>
-    <t>Ninatamani maziwa siki.</t>
-  </si>
-  <si>
-    <t>Babangu anapenda sana matofaa.</t>
-  </si>
-  <si>
-    <t>Minapenda machungwa.</t>
-  </si>
-  <si>
-    <t>Babangu anapenda mkate wa siagi.
-Mimi napenda mkate we sinia.</t>
-  </si>
-  <si>
-    <t>You are free to download, copy, translate or adapt this story and use the illustrations as long as you attribute in the following way:
-Kifungua Kinywa
-Author -
-Clare Verbeek, Thembani Dladla and Zanele Buthelezi
-Translation -
-Fatma Baraka
-Illustration -
-Cathy Feek
-Language -
-Kiswahili
-Level -
-First words
-© School of Education and Development (Centre for Adult Education), University of Kwazulu-Natal 2007
-Creative Commons: Attribution-Non Commercial 3.0
-Source
-www.africanstorybook.org
-Original source
-http://cae.ukzn.ac.za/resources/seedbooks.aspx</t>
-  </si>
-  <si>
     <t>asb/18699.png</t>
   </si>
   <si>
@@ -10999,156 +10946,101 @@
     <t>Monkey and the Drought</t>
   </si>
   <si>
-    <t>Kima na kiangazi</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Alice Edui
  Salim Kasamba</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ursula Nafula
- Salim Kasamba</t>
-  </si>
-  <si>
     <t>asb/18786.png</t>
   </si>
   <si>
     <t>There was severe drought across the land. Bushes and trees dried up. Rivers stopped flowing. There was no water and no food. People,  cattle and wild animals grew thin.</t>
   </si>
   <si>
-    <t>Hapo kale kiangazi kilienea nchi nzima. Miti ilisinyaa. Mito ilikauka. Watu na mifugo wakakosa maji na chakula. Walikonda sana.</t>
-  </si>
-  <si>
     <t>asb/18788.png</t>
   </si>
   <si>
     <t>Many of the monkeys who lived in the hills died of hunger. One day,  a female monkey decided to look for a place where there was no drought.</t>
   </si>
   <si>
-    <t>Kima wengi walioishi milimani walikufa kwa njaa. Siku moja Kima mmoja wa kike alitaka kutafuta suluhu. Alienda kutafuta sehemu isiyo na kiangazi.</t>
-  </si>
-  <si>
     <t>asb/18789.png</t>
   </si>
   <si>
     <t>Monkey travelled for many days. She passed bushes,  climbed hills,  and crossed valleys.</t>
   </si>
   <si>
-    <t>Alisafiri kwa siku nyingi. Alipita vichaka, akapanda milima na kuvuka mabonde.</t>
-  </si>
-  <si>
     <t>asb/18790.png</t>
   </si>
   <si>
     <t>Finally,  Monkey arrived at a place called Tirkol.</t>
   </si>
   <si>
-    <t>Hatimaye, Kima huyo alifika mahali palipoitwa Tirkol.</t>
-  </si>
-  <si>
     <t>asb/18791.png</t>
   </si>
   <si>
     <t>At Tirkol,  Monkey found different kinds of fruit and a flowing river. She was very happy.</t>
   </si>
   <si>
-    <t>Alipata matunda aina nyingi na mto uliobubujika maji. Alifurahi sana.</t>
-  </si>
-  <si>
     <t>asb/18792.png</t>
   </si>
   <si>
     <t>Monkey stayed there. She ate plenty of fruit. She grew fat and shiny. She swam in the river every day.</t>
   </si>
   <si>
-    <t>Kima yule alipiga kambi hapo. Alikula matunda mengi. Akanona na kumetameta. Kwa furaha aliogelea mtoni kila siku.</t>
-  </si>
-  <si>
     <t>asb/18793.png</t>
   </si>
   <si>
     <t>After some time,  Monkey decided to return to the hills. She wanted to see who had survived the drought. She took fruit and followed the path she had used before.</t>
   </si>
   <si>
-    <t>Baada ya muda, aliamua kurudi milimani. Alitaka kujua walionusurika na athari za kiangazi. Alibeba matunda mengi akipitia njia aliyoitumia awali.</t>
-  </si>
-  <si>
     <t>asb/18794.png</t>
   </si>
   <si>
     <t>When she reached the hills,  the surviving monkeys came to welcome her.</t>
   </si>
   <si>
-    <t>Alipofika milimani, kima walionusurika walimlaki.</t>
-  </si>
-  <si>
     <t>asb/18795.png</t>
   </si>
   <si>
     <t>Everyone wanted the fruit she brought. They asked her,  "Where is this wonderful place? We want to go there too."</t>
   </si>
   <si>
-    <t>Kila mmoja wao aliyataka yale matunda aliyoyaleta. Walimwuliza, "Ni sehemu gani iliyo nzuri hivi? Tupeleke pia nasi."</t>
-  </si>
-  <si>
     <t>Monkey told them about the goodness of Tirkol and agreed to take them there.</t>
   </si>
   <si>
-    <t>Kima aliwaelezea uzuri wa Tirkol. Akakubali kuwapeleka huko.</t>
-  </si>
-  <si>
     <t>asb/18797.png</t>
   </si>
   <si>
     <t>All the monkeys moved to Tirkol. They ate fruit,  drank water,  rested and grew fat. They swore never to return to the hills.</t>
   </si>
   <si>
-    <t>Kima wote walihamia Tirkol. Walikula matunda,  wakanywa maji, wakapumzika na wakanona. Wakaapa kutorudi milimani tena.</t>
-  </si>
-  <si>
     <t>asb/18798.png</t>
   </si>
   <si>
     <t>The monkeys who lived in Tirkol soon discovered that monkeys from the hills had moved to their territory.</t>
   </si>
   <si>
-    <t>Punde, kima wenyeji wa Tirkol waligundua kwamba kima wa milimani walikuwa wamehamia sehemu yao.</t>
-  </si>
-  <si>
     <t>asb/18799.png</t>
   </si>
   <si>
     <t>The Tirkol monkeys worried that the fruit would disappear. So they decided to chase away the monkeys from the hills.</t>
   </si>
   <si>
-    <t>Walihofia kuwa matunda hayangewatosha. Wakaamua kuwafukuza kima waliotoka milimani.</t>
-  </si>
-  <si>
     <t>asb/18800.png</t>
   </si>
   <si>
     <t>One day,  the monkeys from the hills were at the river drinking water. The Tirkol monkeys attacked them with canes. They wanted to chase them away.</t>
   </si>
   <si>
-    <t>Siku moja kima wa milimani walikuwa mtoni wakinywa maji. Kima wa Tirkol waliwavamia kwa mijeledi. Walitaka kuwachapa na kuwafukuza.</t>
-  </si>
-  <si>
     <t>asb/18801.png</t>
   </si>
   <si>
     <t>But just before they started fighting,  an elderly monkey hung down from a branch. He asked the monkeys,  "Why do you want to fight? There is enough food for all of us."</t>
   </si>
   <si>
-    <t>Kabla ya vita kuanza, kima mmoja mzee aliwauliza, "Mbona mnataka kupigana? Mimi naona kuna chakula cha kututosha sote."</t>
-  </si>
-  <si>
     <t>asb/18802.png</t>
   </si>
   <si>
     <t>All the monkeys realised that this was true. And so,  since that day,  monkeys from the hills and monkeys from Tirkol have lived together without fighting.</t>
-  </si>
-  <si>
-    <t>Tangu siku hiyo, kima wa kutoka milimani na wale wa Tirkol wamekuwa wakiishi pamoja kwa amani.</t>
   </si>
   <si>
     <t>You are free to download, copy, translate or adapt this story and use the illustrations as long as you attribute in the following way:
@@ -11159,24 +11051,6 @@
 Salim Kasamba
 Language -
 English
-Level -
-First paragraphs
-© African Storybook Initiative 2016
-Creative Commons: Attribution 4.0
-Source
-www.africanstorybook.org</t>
-  </si>
-  <si>
-    <t>You are free to download, copy, translate or adapt this story and use the illustrations as long as you attribute in the following way:
-Kima na kiangazi
-Author -
-Alice Edui
-Translation -
-Ursula Nafula
-Illustration -
-Salim Kasamba
-Language -
-Kiswahili
 Level -
 First paragraphs
 © African Storybook Initiative 2016
@@ -13342,800 +13216,6 @@
 </file>
 
 <file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6500-000000000000}">
-  <dimension ref="A1:G18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3037</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3038</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3039</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3040</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3041</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3042</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3043</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3044</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3045</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3046</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3047</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3048</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3049</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3050</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3051</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3052</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3053</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3054</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3055</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3056</v>
-      </c>
-      <c r="F8" t="s">
-        <v>3057</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3058</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3059</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3060</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3061</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3062</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3063</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3064</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3065</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3066</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3067</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3068</v>
-      </c>
-      <c r="E13" t="s">
-        <v>3069</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3070</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3071</v>
-      </c>
-      <c r="E14" t="s">
-        <v>3072</v>
-      </c>
-      <c r="F14" t="s">
-        <v>3073</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3074</v>
-      </c>
-      <c r="F15" t="s">
-        <v>3075</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3076</v>
-      </c>
-      <c r="E16" t="s">
-        <v>3077</v>
-      </c>
-      <c r="F16" t="s">
-        <v>3078</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3079</v>
-      </c>
-      <c r="E17" t="s">
-        <v>3080</v>
-      </c>
-      <c r="F17" t="s">
-        <v>3081</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
-        <v>3082</v>
-      </c>
-      <c r="F18" t="s">
-        <v>3083</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6600-000000000000}">
-  <dimension ref="A1:G15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3084</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3085</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3086</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3087</v>
-      </c>
-      <c r="F2" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3084</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3088</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3089</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3090</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3091</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3092</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3093</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3094</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3095</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3096</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3097</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3098</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3099</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3100</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3102</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3103</v>
-      </c>
-      <c r="F8" t="s">
-        <v>3104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3105</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3106</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3108</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3109</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3111</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3112</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3114</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3115</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3117</v>
-      </c>
-      <c r="E13" t="s">
-        <v>3118</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3120</v>
-      </c>
-      <c r="E14" t="s">
-        <v>3121</v>
-      </c>
-      <c r="F14" t="s">
-        <v>3122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>3123</v>
-      </c>
-      <c r="F15" t="s">
-        <v>3124</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6700-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6800-000000000000}">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3125</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3126</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3127</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3128</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3130</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3131</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3133</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3134</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3136</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3137</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3139</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3140</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3125</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3142</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3144</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3145</v>
-      </c>
-      <c r="F8" t="s">
-        <v>3146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3147</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3148</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3150</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3151</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3153</v>
-      </c>
-      <c r="E11" t="s">
-        <v>3154</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3156</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3157</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3159</v>
-      </c>
-      <c r="E13" t="s">
-        <v>3160</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3162</v>
-      </c>
-      <c r="E14" t="s">
-        <v>3163</v>
-      </c>
-      <c r="F14" t="s">
-        <v>3164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3165</v>
-      </c>
-      <c r="E15" t="s">
-        <v>3166</v>
-      </c>
-      <c r="F15" t="s">
-        <v>3167</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3168</v>
-      </c>
-      <c r="E16" t="s">
-        <v>3169</v>
-      </c>
-      <c r="F16" t="s">
-        <v>3170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3171</v>
-      </c>
-      <c r="E17" t="s">
-        <v>3172</v>
-      </c>
-      <c r="F17" t="s">
-        <v>3173</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3174</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>3175</v>
-      </c>
-      <c r="F19" t="s">
-        <v>3176</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6900-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -14171,19 +13251,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>3177</v>
+        <v>3148</v>
       </c>
       <c r="C2" t="s">
-        <v>3178</v>
+        <v>3149</v>
       </c>
       <c r="D2" t="s">
-        <v>3179</v>
+        <v>3150</v>
       </c>
       <c r="E2" t="s">
-        <v>3180</v>
+        <v>3151</v>
       </c>
       <c r="F2" t="s">
-        <v>3181</v>
+        <v>3152</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -14191,13 +13271,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>3182</v>
+        <v>3153</v>
       </c>
       <c r="E3" t="s">
-        <v>3183</v>
+        <v>3154</v>
       </c>
       <c r="F3" t="s">
-        <v>3184</v>
+        <v>3155</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -14205,13 +13285,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>3177</v>
+        <v>3148</v>
       </c>
       <c r="E4" t="s">
-        <v>3185</v>
+        <v>3156</v>
       </c>
       <c r="F4" t="s">
-        <v>3186</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -14219,13 +13299,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>3187</v>
+        <v>3158</v>
       </c>
       <c r="E5" t="s">
-        <v>3188</v>
+        <v>3159</v>
       </c>
       <c r="F5" t="s">
-        <v>3189</v>
+        <v>3160</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -14233,13 +13313,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>3190</v>
+        <v>3161</v>
       </c>
       <c r="E6" t="s">
-        <v>3191</v>
+        <v>3162</v>
       </c>
       <c r="F6" t="s">
-        <v>3192</v>
+        <v>3163</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -14247,13 +13327,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>3193</v>
+        <v>3164</v>
       </c>
       <c r="E7" t="s">
-        <v>3194</v>
+        <v>3165</v>
       </c>
       <c r="F7" t="s">
-        <v>3195</v>
+        <v>3166</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -14261,13 +13341,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>3196</v>
+        <v>3167</v>
       </c>
       <c r="E8" t="s">
-        <v>3197</v>
+        <v>3168</v>
       </c>
       <c r="F8" t="s">
-        <v>3198</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -14275,13 +13355,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>3199</v>
+        <v>3170</v>
       </c>
       <c r="E9" t="s">
-        <v>3200</v>
+        <v>3171</v>
       </c>
       <c r="F9" t="s">
-        <v>3201</v>
+        <v>3172</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -14289,13 +13369,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>3202</v>
+        <v>3173</v>
       </c>
       <c r="E10" t="s">
-        <v>3203</v>
+        <v>3174</v>
       </c>
       <c r="F10" t="s">
-        <v>3204</v>
+        <v>3175</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -14303,10 +13383,10 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>3205</v>
+        <v>3176</v>
       </c>
       <c r="F11" t="s">
-        <v>3206</v>
+        <v>3177</v>
       </c>
     </row>
   </sheetData>
@@ -15685,7 +14765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -30708,7 +29788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5800-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -30884,8 +29966,8 @@
 </file>
 
 <file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5900-000000000000}">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5C00-000000000000}">
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -30919,19 +30001,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>2721</v>
+        <v>2750</v>
       </c>
       <c r="C2" t="s">
-        <v>2722</v>
+        <v>2751</v>
       </c>
       <c r="D2" t="s">
-        <v>2750</v>
+        <v>2752</v>
       </c>
       <c r="E2" t="s">
-        <v>821</v>
+        <v>2753</v>
       </c>
       <c r="F2" t="s">
-        <v>2751</v>
+        <v>2754</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -30939,13 +30021,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>2725</v>
+        <v>2755</v>
       </c>
       <c r="E3" t="s">
-        <v>2726</v>
+        <v>2756</v>
       </c>
       <c r="F3" t="s">
-        <v>2752</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -30953,13 +30035,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>2728</v>
+        <v>2758</v>
       </c>
       <c r="E4" t="s">
-        <v>2729</v>
+        <v>2759</v>
       </c>
       <c r="F4" t="s">
-        <v>2753</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -30967,13 +30049,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>2731</v>
+        <v>2761</v>
       </c>
       <c r="E5" t="s">
-        <v>2732</v>
+        <v>2762</v>
       </c>
       <c r="F5" t="s">
-        <v>2754</v>
+        <v>2763</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -30981,13 +30063,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>2734</v>
+        <v>2750</v>
       </c>
       <c r="E6" t="s">
-        <v>2735</v>
+        <v>2764</v>
       </c>
       <c r="F6" t="s">
-        <v>2755</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -30995,13 +30077,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>2737</v>
+        <v>2766</v>
       </c>
       <c r="E7" t="s">
-        <v>2738</v>
+        <v>2767</v>
       </c>
       <c r="F7" t="s">
-        <v>2756</v>
+        <v>2768</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -31009,13 +30091,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>2740</v>
+        <v>2769</v>
       </c>
       <c r="E8" t="s">
-        <v>2741</v>
+        <v>2770</v>
       </c>
       <c r="F8" t="s">
-        <v>2757</v>
+        <v>2771</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -31023,13 +30105,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>2721</v>
+        <v>2772</v>
       </c>
       <c r="E9" t="s">
-        <v>2743</v>
+        <v>2773</v>
       </c>
       <c r="F9" t="s">
-        <v>2758</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -31037,24 +30119,80 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>2745</v>
+        <v>2775</v>
       </c>
       <c r="E10" t="s">
-        <v>2746</v>
+        <v>2776</v>
       </c>
       <c r="F10" t="s">
-        <v>2747</v>
+        <v>2777</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
+      <c r="B11" t="s">
+        <v>2778</v>
+      </c>
       <c r="E11" t="s">
-        <v>2748</v>
+        <v>2779</v>
       </c>
       <c r="F11" t="s">
-        <v>2759</v>
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2781</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2782</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2784</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2785</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2786</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2787</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2788</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2789</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2790</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2791</v>
       </c>
     </row>
   </sheetData>
@@ -31063,13 +30201,292 @@
 </file>
 
 <file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5A00-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5E00-000000000000}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2792</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2793</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2827</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2794</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2828</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2795</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2796</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2829</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2798</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2799</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2800</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2831</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2801</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2802</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2832</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2803</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2804</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2805</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2806</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2834</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2807</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2808</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2835</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2809</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2810</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2836</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2811</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2812</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2837</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2792</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2813</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2838</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2814</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2815</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2839</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2816</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2817</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2818</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2819</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2841</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2820</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2821</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2842</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2822</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2823</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2843</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2824</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2825</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2844</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2826</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2845</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -31087,835 +30504,6 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5B00-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5C00-000000000000}">
-  <dimension ref="A1:G15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2760</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2761</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2762</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2763</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2764</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2765</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2766</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2767</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2768</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2769</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2770</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2771</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2772</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2773</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2760</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2774</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2775</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2776</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2777</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2778</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2779</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2780</v>
-      </c>
-      <c r="F8" t="s">
-        <v>2781</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2782</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2783</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2784</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2785</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2786</v>
-      </c>
-      <c r="F10" t="s">
-        <v>2787</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2788</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2789</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2790</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2791</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2792</v>
-      </c>
-      <c r="F12" t="s">
-        <v>2793</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2794</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2795</v>
-      </c>
-      <c r="F13" t="s">
-        <v>2796</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2797</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2798</v>
-      </c>
-      <c r="F14" t="s">
-        <v>2799</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2800</v>
-      </c>
-      <c r="F15" t="s">
-        <v>2801</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5D00-000000000000}">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2802</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2803</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2804</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2805</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2806</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2807</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2808</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2809</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2810</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2811</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2812</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2813</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2814</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2815</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2816</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2817</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2818</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2819</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2820</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2821</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2822</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2823</v>
-      </c>
-      <c r="F8" t="s">
-        <v>2824</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2825</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2826</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2827</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2828</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2829</v>
-      </c>
-      <c r="F10" t="s">
-        <v>2830</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2831</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2832</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2833</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2802</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2834</v>
-      </c>
-      <c r="F12" t="s">
-        <v>2835</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2836</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2837</v>
-      </c>
-      <c r="F13" t="s">
-        <v>2838</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2839</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2840</v>
-      </c>
-      <c r="F14" t="s">
-        <v>2841</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2842</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2843</v>
-      </c>
-      <c r="F15" t="s">
-        <v>2844</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2845</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2846</v>
-      </c>
-      <c r="F16" t="s">
-        <v>2847</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2848</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2849</v>
-      </c>
-      <c r="F17" t="s">
-        <v>2850</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2851</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2852</v>
-      </c>
-      <c r="F18" t="s">
-        <v>2853</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2854</v>
-      </c>
-      <c r="F19" t="s">
-        <v>2855</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5E00-000000000000}">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2802</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2803</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2856</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2805</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2857</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2807</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2808</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2858</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2810</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2811</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2859</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2813</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2814</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2860</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2816</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2817</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2861</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2819</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2820</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2862</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2822</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2823</v>
-      </c>
-      <c r="F8" t="s">
-        <v>2863</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2825</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2826</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2864</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2828</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2829</v>
-      </c>
-      <c r="F10" t="s">
-        <v>2865</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2831</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2832</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2866</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2802</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2834</v>
-      </c>
-      <c r="F12" t="s">
-        <v>2867</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2836</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2837</v>
-      </c>
-      <c r="F13" t="s">
-        <v>2868</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2839</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2840</v>
-      </c>
-      <c r="F14" t="s">
-        <v>2869</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2842</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2843</v>
-      </c>
-      <c r="F15" t="s">
-        <v>2870</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2845</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2846</v>
-      </c>
-      <c r="F16" t="s">
-        <v>2871</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2848</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2849</v>
-      </c>
-      <c r="F17" t="s">
-        <v>2872</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2851</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2852</v>
-      </c>
-      <c r="F18" t="s">
-        <v>2873</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2854</v>
-      </c>
-      <c r="F19" t="s">
-        <v>2874</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5F00-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
@@ -31951,19 +30539,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>2875</v>
+        <v>2846</v>
       </c>
       <c r="C2" t="s">
-        <v>2876</v>
+        <v>2847</v>
       </c>
       <c r="D2" t="s">
-        <v>2877</v>
+        <v>2848</v>
       </c>
       <c r="E2" t="s">
-        <v>2878</v>
+        <v>2849</v>
       </c>
       <c r="F2" t="s">
-        <v>2879</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -31971,13 +30559,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>2880</v>
+        <v>2851</v>
       </c>
       <c r="E3" t="s">
-        <v>2881</v>
+        <v>2852</v>
       </c>
       <c r="F3" t="s">
-        <v>2882</v>
+        <v>2853</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -31985,13 +30573,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>2883</v>
+        <v>2854</v>
       </c>
       <c r="E4" t="s">
-        <v>2884</v>
+        <v>2855</v>
       </c>
       <c r="F4" t="s">
-        <v>2885</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -31999,13 +30587,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>2886</v>
+        <v>2857</v>
       </c>
       <c r="E5" t="s">
-        <v>2887</v>
+        <v>2858</v>
       </c>
       <c r="F5" t="s">
-        <v>2888</v>
+        <v>2859</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -32013,13 +30601,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>2889</v>
+        <v>2860</v>
       </c>
       <c r="E6" t="s">
-        <v>2890</v>
+        <v>2861</v>
       </c>
       <c r="F6" t="s">
-        <v>2891</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -32027,13 +30615,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>2892</v>
+        <v>2863</v>
       </c>
       <c r="E7" t="s">
-        <v>2893</v>
+        <v>2864</v>
       </c>
       <c r="F7" t="s">
-        <v>2894</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -32041,13 +30629,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>2895</v>
+        <v>2866</v>
       </c>
       <c r="E8" t="s">
-        <v>2896</v>
+        <v>2867</v>
       </c>
       <c r="F8" t="s">
-        <v>2897</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -32055,13 +30643,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>2898</v>
+        <v>2869</v>
       </c>
       <c r="E9" t="s">
-        <v>2899</v>
+        <v>2870</v>
       </c>
       <c r="F9" t="s">
-        <v>2900</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -32069,13 +30657,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>2901</v>
+        <v>2872</v>
       </c>
       <c r="E10" t="s">
-        <v>2902</v>
+        <v>2873</v>
       </c>
       <c r="F10" t="s">
-        <v>2903</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -32083,13 +30671,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>2904</v>
+        <v>2875</v>
       </c>
       <c r="E11" t="s">
-        <v>2905</v>
+        <v>2876</v>
       </c>
       <c r="F11" t="s">
-        <v>2906</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -32097,13 +30685,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>2907</v>
+        <v>2878</v>
       </c>
       <c r="E12" t="s">
-        <v>2908</v>
+        <v>2879</v>
       </c>
       <c r="F12" t="s">
-        <v>2909</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -32111,13 +30699,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>2910</v>
+        <v>2881</v>
       </c>
       <c r="E13" t="s">
-        <v>2911</v>
+        <v>2882</v>
       </c>
       <c r="F13" t="s">
-        <v>2912</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -32125,13 +30713,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>2913</v>
+        <v>2884</v>
       </c>
       <c r="E14" t="s">
-        <v>2914</v>
+        <v>2885</v>
       </c>
       <c r="F14" t="s">
-        <v>2915</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -32139,13 +30727,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>2916</v>
+        <v>2887</v>
       </c>
       <c r="E15" t="s">
-        <v>2917</v>
+        <v>2888</v>
       </c>
       <c r="F15" t="s">
-        <v>2918</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -32153,13 +30741,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>2919</v>
+        <v>2890</v>
       </c>
       <c r="E16" t="s">
-        <v>2920</v>
+        <v>2891</v>
       </c>
       <c r="F16" t="s">
-        <v>2921</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -32167,13 +30755,13 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>2922</v>
+        <v>2893</v>
       </c>
       <c r="E17" t="s">
-        <v>2923</v>
+        <v>2894</v>
       </c>
       <c r="F17" t="s">
-        <v>2924</v>
+        <v>2895</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -32181,13 +30769,13 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>2875</v>
+        <v>2846</v>
       </c>
       <c r="E18" t="s">
-        <v>2925</v>
+        <v>2896</v>
       </c>
       <c r="F18" t="s">
-        <v>2926</v>
+        <v>2897</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -32195,10 +30783,10 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>2927</v>
+        <v>2898</v>
       </c>
       <c r="F19" t="s">
-        <v>2928</v>
+        <v>2899</v>
       </c>
     </row>
   </sheetData>
@@ -32206,7 +30794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -32242,19 +30830,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>2929</v>
+        <v>2900</v>
       </c>
       <c r="C2" t="s">
-        <v>2930</v>
+        <v>2901</v>
       </c>
       <c r="D2" t="s">
-        <v>2931</v>
+        <v>2902</v>
       </c>
       <c r="E2" t="s">
-        <v>2932</v>
+        <v>2903</v>
       </c>
       <c r="F2" t="s">
-        <v>2933</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -32262,13 +30850,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>2929</v>
+        <v>2900</v>
       </c>
       <c r="E3" t="s">
-        <v>2934</v>
+        <v>2905</v>
       </c>
       <c r="F3" t="s">
-        <v>2935</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -32276,13 +30864,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>2936</v>
+        <v>2907</v>
       </c>
       <c r="E4" t="s">
-        <v>2937</v>
+        <v>2908</v>
       </c>
       <c r="F4" t="s">
-        <v>2938</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -32290,13 +30878,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>2939</v>
+        <v>2910</v>
       </c>
       <c r="E5" t="s">
-        <v>2940</v>
+        <v>2911</v>
       </c>
       <c r="F5" t="s">
-        <v>2941</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -32304,13 +30892,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>2942</v>
+        <v>2913</v>
       </c>
       <c r="E6" t="s">
-        <v>2943</v>
+        <v>2914</v>
       </c>
       <c r="F6" t="s">
-        <v>2944</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -32318,13 +30906,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>2945</v>
+        <v>2916</v>
       </c>
       <c r="E7" t="s">
-        <v>2946</v>
+        <v>2917</v>
       </c>
       <c r="F7" t="s">
-        <v>2947</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -32332,13 +30920,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>2948</v>
+        <v>2919</v>
       </c>
       <c r="E8" t="s">
-        <v>2949</v>
+        <v>2920</v>
       </c>
       <c r="F8" t="s">
-        <v>2950</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -32346,13 +30934,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>2951</v>
+        <v>2922</v>
       </c>
       <c r="E9" t="s">
-        <v>2952</v>
+        <v>2923</v>
       </c>
       <c r="F9" t="s">
-        <v>2953</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -32360,13 +30948,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>2954</v>
+        <v>2925</v>
       </c>
       <c r="E10" t="s">
-        <v>2955</v>
+        <v>2926</v>
       </c>
       <c r="F10" t="s">
-        <v>2956</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -32374,13 +30962,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>2957</v>
+        <v>2928</v>
       </c>
       <c r="E11" t="s">
-        <v>2958</v>
+        <v>2929</v>
       </c>
       <c r="F11" t="s">
-        <v>2959</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -32388,13 +30976,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>2960</v>
+        <v>2931</v>
       </c>
       <c r="E12" t="s">
-        <v>2961</v>
+        <v>2932</v>
       </c>
       <c r="F12" t="s">
-        <v>2962</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -32402,10 +30990,10 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>2963</v>
+        <v>2934</v>
       </c>
       <c r="F13" t="s">
-        <v>2964</v>
+        <v>2935</v>
       </c>
     </row>
   </sheetData>
@@ -32413,7 +31001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -32425,7 +31013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6200-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -32461,19 +31049,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>2965</v>
+        <v>2936</v>
       </c>
       <c r="C2" t="s">
-        <v>2966</v>
+        <v>2937</v>
       </c>
       <c r="D2" t="s">
-        <v>2967</v>
+        <v>2938</v>
       </c>
       <c r="E2" t="s">
-        <v>2968</v>
+        <v>2939</v>
       </c>
       <c r="F2" t="s">
-        <v>2969</v>
+        <v>2940</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -32481,13 +31069,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>2965</v>
+        <v>2936</v>
       </c>
       <c r="E3" t="s">
-        <v>2970</v>
+        <v>2941</v>
       </c>
       <c r="F3" t="s">
-        <v>2971</v>
+        <v>2942</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -32495,13 +31083,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>2972</v>
+        <v>2943</v>
       </c>
       <c r="E4" t="s">
-        <v>2973</v>
+        <v>2944</v>
       </c>
       <c r="F4" t="s">
-        <v>2974</v>
+        <v>2945</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -32509,13 +31097,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>2975</v>
+        <v>2946</v>
       </c>
       <c r="E5" t="s">
-        <v>2976</v>
+        <v>2947</v>
       </c>
       <c r="F5" t="s">
-        <v>2977</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -32523,13 +31111,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>2978</v>
+        <v>2949</v>
       </c>
       <c r="E6" t="s">
-        <v>2979</v>
+        <v>2950</v>
       </c>
       <c r="F6" t="s">
-        <v>2980</v>
+        <v>2951</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -32537,13 +31125,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>2981</v>
+        <v>2952</v>
       </c>
       <c r="E7" t="s">
-        <v>2982</v>
+        <v>2953</v>
       </c>
       <c r="F7" t="s">
-        <v>2983</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -32551,13 +31139,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>2984</v>
+        <v>2955</v>
       </c>
       <c r="E8" t="s">
-        <v>2985</v>
+        <v>2956</v>
       </c>
       <c r="F8" t="s">
-        <v>2986</v>
+        <v>2957</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -32565,13 +31153,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>2987</v>
+        <v>2958</v>
       </c>
       <c r="E9" t="s">
-        <v>2988</v>
+        <v>2959</v>
       </c>
       <c r="F9" t="s">
-        <v>2989</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -32579,13 +31167,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>2990</v>
+        <v>2961</v>
       </c>
       <c r="E10" t="s">
-        <v>2991</v>
+        <v>2962</v>
       </c>
       <c r="F10" t="s">
-        <v>2992</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -32593,10 +31181,10 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>2993</v>
+        <v>2964</v>
       </c>
       <c r="F11" t="s">
-        <v>2994</v>
+        <v>2965</v>
       </c>
     </row>
   </sheetData>
@@ -32604,7 +31192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6300-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -32640,19 +31228,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>2995</v>
+        <v>2966</v>
       </c>
       <c r="C2" t="s">
-        <v>2996</v>
+        <v>2967</v>
       </c>
       <c r="D2" t="s">
-        <v>2997</v>
+        <v>2968</v>
       </c>
       <c r="E2" t="s">
-        <v>2998</v>
+        <v>2969</v>
       </c>
       <c r="F2" t="s">
-        <v>2999</v>
+        <v>2970</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -32660,13 +31248,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>3000</v>
+        <v>2971</v>
       </c>
       <c r="E3" t="s">
-        <v>3001</v>
+        <v>2972</v>
       </c>
       <c r="F3" t="s">
-        <v>3002</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -32674,13 +31262,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>3003</v>
+        <v>2974</v>
       </c>
       <c r="E4" t="s">
-        <v>3004</v>
+        <v>2975</v>
       </c>
       <c r="F4" t="s">
-        <v>3005</v>
+        <v>2976</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -32688,13 +31276,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>3006</v>
+        <v>2977</v>
       </c>
       <c r="E5" t="s">
-        <v>3007</v>
+        <v>2978</v>
       </c>
       <c r="F5" t="s">
-        <v>3008</v>
+        <v>2979</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -32702,13 +31290,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>2995</v>
+        <v>2966</v>
       </c>
       <c r="E6" t="s">
-        <v>3009</v>
+        <v>2980</v>
       </c>
       <c r="F6" t="s">
-        <v>3010</v>
+        <v>2981</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -32716,13 +31304,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>3011</v>
+        <v>2982</v>
       </c>
       <c r="E7" t="s">
-        <v>3012</v>
+        <v>2983</v>
       </c>
       <c r="F7" t="s">
-        <v>3013</v>
+        <v>2984</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -32730,13 +31318,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>3014</v>
+        <v>2985</v>
       </c>
       <c r="E8" t="s">
-        <v>3015</v>
+        <v>2986</v>
       </c>
       <c r="F8" t="s">
-        <v>3016</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -32744,13 +31332,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>3017</v>
+        <v>2988</v>
       </c>
       <c r="E9" t="s">
-        <v>3018</v>
+        <v>2989</v>
       </c>
       <c r="F9" t="s">
-        <v>3019</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -32758,13 +31346,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>3020</v>
+        <v>2991</v>
       </c>
       <c r="E10" t="s">
-        <v>3021</v>
+        <v>2992</v>
       </c>
       <c r="F10" t="s">
-        <v>3022</v>
+        <v>2993</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -32772,13 +31360,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>3023</v>
+        <v>2994</v>
       </c>
       <c r="E11" t="s">
-        <v>3024</v>
+        <v>2995</v>
       </c>
       <c r="F11" t="s">
-        <v>3025</v>
+        <v>2996</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -32786,13 +31374,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>3026</v>
+        <v>2997</v>
       </c>
       <c r="E12" t="s">
-        <v>3027</v>
+        <v>2998</v>
       </c>
       <c r="F12" t="s">
-        <v>3028</v>
+        <v>2999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -32800,13 +31388,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>3029</v>
+        <v>3000</v>
       </c>
       <c r="E13" t="s">
-        <v>3030</v>
+        <v>3001</v>
       </c>
       <c r="F13" t="s">
-        <v>3031</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -32814,13 +31402,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>3032</v>
+        <v>3003</v>
       </c>
       <c r="E14" t="s">
-        <v>3033</v>
+        <v>3004</v>
       </c>
       <c r="F14" t="s">
-        <v>3034</v>
+        <v>3005</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -32828,10 +31416,10 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>3035</v>
+        <v>3006</v>
       </c>
       <c r="F15" t="s">
-        <v>3036</v>
+        <v>3007</v>
       </c>
     </row>
   </sheetData>
@@ -32839,7 +31427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -32849,4 +31437,798 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6500-000000000000}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3008</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3009</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3010</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3011</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3013</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3014</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3016</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3018</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3019</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3021</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3023</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3024</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3026</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3027</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3029</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3031</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3032</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3034</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3035</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3036</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3037</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3039</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3040</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3041</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3042</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3043</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3044</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3045</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3047</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3048</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3049</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3050</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3051</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3052</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3053</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6600-000000000000}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3055</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3056</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3057</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3058</v>
+      </c>
+      <c r="F2" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3055</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3059</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3061</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3062</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3063</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3064</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3065</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3067</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3068</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3070</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3071</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3073</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3074</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3076</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3077</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3078</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3079</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3080</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3081</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3082</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3083</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3084</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3085</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3086</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3088</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3089</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3091</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3092</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3094</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3095</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6700-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6800-000000000000}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3096</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3098</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3099</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3102</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3104</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3105</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3107</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3108</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3110</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3096</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3115</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3116</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3118</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3119</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3121</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3122</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3125</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3127</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3128</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3130</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3131</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3133</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3134</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3136</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3137</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3139</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3140</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3142</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3143</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3146</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>